<commit_message>
PART 3 COMPLETED. All test pass, our and hers
</commit_message>
<xml_diff>
--- a/ClueBoard/boardConfigTestSheet.xlsx
+++ b/ClueBoard/boardConfigTestSheet.xlsx
@@ -265,7 +265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,12 +472,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,23 +678,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1043,11 +1036,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1067,7 @@
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1099,7 +1094,7 @@
       <c r="Q1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -1117,8 +1112,11 @@
       <c r="W1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
+      <c r="X1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1126,7 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1188,8 +1186,11 @@
       <c r="W2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="X2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1205,7 +1206,7 @@
       <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1259,8 +1260,11 @@
       <c r="W3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="X3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1330,8 +1334,11 @@
       <c r="W4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="X4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1401,8 +1408,11 @@
       <c r="W5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="X5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1472,8 +1482,11 @@
       <c r="W6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="X6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1543,9 +1556,12 @@
       <c r="W7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="1" t="s">
+      <c r="X7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1590,7 +1606,7 @@
       <c r="O8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="13" t="s">
         <v>1</v>
       </c>
       <c r="Q8" s="1" t="s">
@@ -1614,15 +1630,18 @@
       <c r="W8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="X8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1634,7 +1653,7 @@
       <c r="F9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="14" t="s">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1646,22 +1665,22 @@
       <c r="J9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P9" s="8" t="s">
+      <c r="K9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q9" s="1" t="s">
@@ -1685,8 +1704,11 @@
       <c r="W9" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="X9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1711,31 +1733,31 @@
       <c r="H10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="12" t="s">
+      <c r="K10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="11" t="s">
         <v>1</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -1756,8 +1778,11 @@
       <c r="W10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="X10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1770,7 +1795,7 @@
       <c r="D11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1788,31 +1813,31 @@
       <c r="J11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q11" s="15" t="s">
+      <c r="K11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="14" t="s">
         <v>1</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="11" t="s">
+      <c r="S11" s="10" t="s">
         <v>1</v>
       </c>
       <c r="T11" s="2" t="s">
@@ -1827,9 +1852,12 @@
       <c r="W11" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="13" t="s">
+      <c r="X11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1841,7 +1869,7 @@
       <c r="D12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1859,22 +1887,22 @@
       <c r="J12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P12" s="8" t="s">
+      <c r="K12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="1" t="s">
@@ -1898,8 +1926,11 @@
       <c r="W12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="X12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1930,22 +1961,22 @@
       <c r="J13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P13" s="8" t="s">
+      <c r="K13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q13" s="1" t="s">
@@ -1969,8 +2000,11 @@
       <c r="W13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="X13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -2001,22 +2035,22 @@
       <c r="J14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P14" s="8" t="s">
+      <c r="K14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q14" s="1" t="s">
@@ -2034,15 +2068,18 @@
       <c r="U14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="V14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="W14" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="12" t="s">
+      <c r="X14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2111,8 +2148,11 @@
       <c r="W15" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="X15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -2152,7 +2192,7 @@
       <c r="M16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="N16" s="11" t="s">
         <v>1</v>
       </c>
       <c r="O16" s="1" t="s">
@@ -2179,8 +2219,11 @@
       <c r="V16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="9" t="s">
-        <v>1</v>
+      <c r="W16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -2190,7 +2233,7 @@
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -2199,7 +2242,7 @@
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -2235,7 +2278,7 @@
       <c r="Q17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R17" s="14" t="s">
+      <c r="R17" s="13" t="s">
         <v>1</v>
       </c>
       <c r="S17" s="1" t="s">
@@ -2252,6 +2295,9 @@
       </c>
       <c r="W17" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="X17">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -2306,7 +2352,7 @@
       <c r="Q18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R18" s="11" t="s">
+      <c r="R18" s="10" t="s">
         <v>1</v>
       </c>
       <c r="S18" s="2" t="s">
@@ -2324,6 +2370,9 @@
       <c r="W18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="X18">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="1" t="s">
@@ -2347,7 +2396,7 @@
       <c r="G19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="8" t="s">
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -2395,6 +2444,9 @@
       <c r="W19" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="X19">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="1" t="s">
@@ -2465,6 +2517,9 @@
       </c>
       <c r="W20" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="X20">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -2519,7 +2574,7 @@
       <c r="Q21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R21" s="13" t="s">
+      <c r="R21" s="12" t="s">
         <v>1</v>
       </c>
       <c r="S21" s="2" t="s">
@@ -2536,6 +2591,9 @@
       </c>
       <c r="W21" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="X21">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -2545,7 +2603,7 @@
       <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -2608,7 +2666,80 @@
       <c r="W22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X22" s="5"/>
+      <c r="X22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <v>11</v>
+      </c>
+      <c r="M23">
+        <v>12</v>
+      </c>
+      <c r="N23">
+        <v>13</v>
+      </c>
+      <c r="O23">
+        <v>14</v>
+      </c>
+      <c r="P23">
+        <v>15</v>
+      </c>
+      <c r="Q23">
+        <v>16</v>
+      </c>
+      <c r="R23">
+        <v>17</v>
+      </c>
+      <c r="S23">
+        <v>18</v>
+      </c>
+      <c r="T23">
+        <v>19</v>
+      </c>
+      <c r="U23">
+        <v>20</v>
+      </c>
+      <c r="V23">
+        <v>21</v>
+      </c>
+      <c r="W23">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:24">
       <c r="A25" t="s">
@@ -2641,12 +2772,12 @@
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="6"/>
+      <c r="A32" s="5"/>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">

</xml_diff>